<commit_message>
move file reading to proxy api
</commit_message>
<xml_diff>
--- a/SimpleExcelWebAddIn/bin/Debug/Book1.xlsx
+++ b/SimpleExcelWebAddIn/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re391f9566aa34d2d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re28039cc84d740a5"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rde718c9e091d42af"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ra0f67505282d4679"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2bed2b2e-f5bb-4505-9764-e4ea955b4d35}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ff8b108d-c739-40c7-94ef-9dc4f934f2e7}">
   <we:reference id="3e0c392a-e70e-4244-a674-3207ebcf220d" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>